<commit_message>
Export Themes + Site canvas
</commit_message>
<xml_diff>
--- a/Estimation du temps de travail.xlsx
+++ b/Estimation du temps de travail.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thiba\Documents\Projet\ArrakisNG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1724571-48B3-412B-BA4D-30A994C72ABF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44C6C3E2-D56B-400D-BE48-FE06C2248C23}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Estimations des tâches" sheetId="2" r:id="rId1"/>
@@ -145,9 +145,6 @@
     <t>Couleur</t>
   </si>
   <si>
-    <t>Principale, Scondaire, Sombre</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <b/>
@@ -466,6 +463,9 @@
   </si>
   <si>
     <t>Récupération des entêtes</t>
+  </si>
+  <si>
+    <t>Principale, Scondaire</t>
   </si>
 </sst>
 </file>
@@ -860,475 +860,475 @@
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="18.1796875" style="3" customWidth="1"/>
-    <col min="4" max="4" width="50.90625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="18.08984375" style="8" customWidth="1"/>
+    <col min="3" max="3" width="18.21875" style="3" customWidth="1"/>
+    <col min="4" max="4" width="50.88671875" style="3" customWidth="1"/>
+    <col min="5" max="5" width="18.109375" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="C1" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="D1" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="E1" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="E1" s="7" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>86</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>87</v>
       </c>
       <c r="E2" s="8">
         <v>1.5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>88</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>89</v>
       </c>
       <c r="E3" s="8">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C4" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>91</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>92</v>
       </c>
       <c r="E4" s="8">
         <v>0.2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C5" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>93</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>94</v>
       </c>
       <c r="E5" s="8">
         <v>0.1</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C6" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>95</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>96</v>
       </c>
       <c r="E6" s="8">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C7" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>97</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>98</v>
       </c>
       <c r="E7" s="8">
         <v>0.5</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C8" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>99</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>100</v>
       </c>
       <c r="E8" s="8">
         <v>0.5</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C9" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>103</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>104</v>
       </c>
       <c r="E9" s="8">
         <v>0.7</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C10" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="D10" s="3" t="s">
         <v>105</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>106</v>
       </c>
       <c r="E10" s="8">
         <v>0.3</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E11" s="8">
         <v>0.3</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B12" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C12" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>108</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>109</v>
       </c>
       <c r="E12" s="8">
         <v>0.4</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B13" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E13" s="8">
         <v>0.2</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B14" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E14" s="8">
         <v>0.3</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B15" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E15" s="8">
         <v>0.3</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B16" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C16" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="D16" s="3" t="s">
         <v>113</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>114</v>
       </c>
       <c r="E16" s="8">
         <v>0.6</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B17" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E17" s="8">
         <v>0.5</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B18" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C18" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="D18" s="3" t="s">
         <v>116</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>117</v>
       </c>
       <c r="E18" s="8">
         <v>0.7</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B19" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E19" s="8">
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B20" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E20" s="8">
         <v>0.3</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B21" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C21" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="D21" s="3" t="s">
         <v>120</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>121</v>
       </c>
       <c r="E21" s="8">
         <v>0.8</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B22" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C22" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="D22" s="3" t="s">
         <v>122</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>123</v>
       </c>
       <c r="E22" s="8">
         <v>0.7</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B23" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C23" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="D23" s="3" t="s">
         <v>124</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>125</v>
       </c>
       <c r="E23" s="8">
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B24" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C24" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="D24" s="3" t="s">
         <v>126</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>127</v>
       </c>
       <c r="E24" s="8">
         <v>0.5</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B25" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C25" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="D25" s="3" t="s">
         <v>128</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>129</v>
       </c>
       <c r="E25" s="8">
         <v>0.5</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B26" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C26" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="D26" s="3" t="s">
         <v>130</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>131</v>
       </c>
       <c r="E26" s="8">
         <v>0.5</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B27" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C27" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="D27" s="3" t="s">
         <v>132</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>133</v>
       </c>
       <c r="E27" s="8">
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D29" s="9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E29" s="10">
         <f>SUM(E2:E28)</f>
@@ -1345,18 +1345,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="36" customWidth="1"/>
-    <col min="2" max="2" width="19.1796875" customWidth="1"/>
-    <col min="4" max="4" width="29.54296875" customWidth="1"/>
+    <col min="2" max="2" width="19.21875" customWidth="1"/>
+    <col min="4" max="4" width="29.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -1367,17 +1367,17 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D3" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
@@ -1385,10 +1385,10 @@
         <v>17</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -1396,10 +1396,10 @@
         <v>2</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.35">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -1407,10 +1407,10 @@
         <v>14</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -1418,10 +1418,10 @@
         <v>4</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>16</v>
       </c>
@@ -1429,22 +1429,22 @@
         <v>4</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.35">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10"/>
       <c r="B10"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>19</v>
       </c>
@@ -1452,15 +1452,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B13" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -1468,7 +1468,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>27</v>
       </c>
@@ -1476,7 +1476,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>0</v>
       </c>
@@ -1484,7 +1484,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>1</v>
       </c>
@@ -1492,7 +1492,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>28</v>
       </c>
@@ -1500,7 +1500,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>1</v>
       </c>
@@ -1508,7 +1508,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>23</v>
       </c>
@@ -1516,15 +1516,15 @@
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B24" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -1532,7 +1532,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>30</v>
       </c>
@@ -1540,7 +1540,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>25</v>
       </c>
@@ -1548,7 +1548,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="29" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>26</v>
       </c>
@@ -1556,7 +1556,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>30</v>
       </c>
@@ -1564,7 +1564,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>31</v>
       </c>
@@ -1572,7 +1572,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>32</v>
       </c>
@@ -1580,7 +1580,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>30</v>
       </c>
@@ -1588,15 +1588,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B35" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>34</v>
       </c>
@@ -1604,7 +1604,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>33</v>
       </c>
@@ -1612,27 +1612,27 @@
         <v>21</v>
       </c>
     </row>
-    <row r="39" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B39" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>30</v>
       </c>
@@ -1640,19 +1640,19 @@
         <v>21</v>
       </c>
     </row>
-    <row r="43" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A43"/>
       <c r="B43"/>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>30</v>
       </c>
@@ -1660,27 +1660,27 @@
         <v>21</v>
       </c>
     </row>
-    <row r="46" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A46"/>
       <c r="B46"/>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
         <v>43</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A48" t="s">
-        <v>44</v>
       </c>
       <c r="B48" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="49" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>30</v>
       </c>
@@ -1688,15 +1688,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>30</v>
       </c>
@@ -1704,19 +1704,19 @@
         <v>4</v>
       </c>
     </row>
-    <row r="53" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A53"/>
       <c r="B53"/>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>30</v>
       </c>
@@ -1724,15 +1724,15 @@
         <v>21</v>
       </c>
     </row>
-    <row r="57" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>30</v>
       </c>
@@ -1740,15 +1740,15 @@
         <v>21</v>
       </c>
     </row>
-    <row r="60" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B60" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B60" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>30</v>
       </c>
@@ -1756,24 +1756,24 @@
         <v>21</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B62" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="63" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="64" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="64" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="65" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
         <v>30</v>
       </c>
@@ -1781,55 +1781,55 @@
         <v>22</v>
       </c>
     </row>
-    <row r="67" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="68" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B68" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B72" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B73" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>30</v>
       </c>
@@ -1837,15 +1837,15 @@
         <v>21</v>
       </c>
     </row>
-    <row r="76" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B76" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>30</v>
       </c>
@@ -1853,31 +1853,31 @@
         <v>21</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B78" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B79" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="81" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>30</v>
       </c>
@@ -1885,15 +1885,15 @@
         <v>21</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B83" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
         <v>29</v>
       </c>
@@ -1901,7 +1901,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>5</v>
       </c>
@@ -1909,7 +1909,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>6</v>
       </c>
@@ -1917,7 +1917,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>7</v>
       </c>
@@ -1925,7 +1925,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>8</v>
       </c>
@@ -1933,103 +1933,103 @@
         <v>4</v>
       </c>
     </row>
-    <row r="91" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
         <v>64</v>
-      </c>
-      <c r="B91" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A92" t="s">
-        <v>65</v>
       </c>
       <c r="B92" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B93" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B94" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="96" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A96" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A97" t="s">
         <v>69</v>
-      </c>
-      <c r="B96" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A97" t="s">
-        <v>70</v>
       </c>
       <c r="B97" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B98" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="100" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A100" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B100" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
+        <v>72</v>
+      </c>
+      <c r="B101" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A102" t="s">
         <v>73</v>
-      </c>
-      <c r="B101" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A102" t="s">
-        <v>74</v>
       </c>
       <c r="B102" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="104" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A104" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B104" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B105" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>30</v>
       </c>
@@ -2037,23 +2037,23 @@
         <v>4</v>
       </c>
     </row>
-    <row r="108" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A108" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B108" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B109" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>30</v>
       </c>

</xml_diff>

<commit_message>
Add search on Table
</commit_message>
<xml_diff>
--- a/Estimation du temps de travail.xlsx
+++ b/Estimation du temps de travail.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thiba\Documents\Projet\ArrakisNG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44C6C3E2-D56B-400D-BE48-FE06C2248C23}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3689C03D-3234-48F5-A260-FDC5993B28FB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="139">
   <si>
     <t>Reprise des bords</t>
   </si>
@@ -456,9 +456,6 @@
     <t>Total (en Jour par Homme):</t>
   </si>
   <si>
-    <t>Export des fichiers SCSS + fonction de génération</t>
-  </si>
-  <si>
     <t>Ajout des paramètres(disabled, max/minlenght, resize)</t>
   </si>
   <si>
@@ -466,6 +463,12 @@
   </si>
   <si>
     <t>Principale, Scondaire</t>
+  </si>
+  <si>
+    <t>Export des fichiers SCSS + fonction de génération de thème</t>
+  </si>
+  <si>
+    <t>Fonction de tri et de recherche</t>
   </si>
 </sst>
 </file>
@@ -856,8 +859,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C333308-878C-4B2F-BAD6-3AA713D341C0}">
   <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -915,7 +918,7 @@
         <v>88</v>
       </c>
       <c r="E3" s="8">
-        <v>2</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -966,7 +969,7 @@
         <v>95</v>
       </c>
       <c r="E6" s="8">
-        <v>1</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -1343,10 +1346,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D110"/>
+  <dimension ref="A1:D111"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1374,7 +1377,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -1441,7 +1444,7 @@
         <v>18</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>66</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -1454,7 +1457,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="B13" t="s">
         <v>17</v>
@@ -1513,12 +1516,12 @@
         <v>23</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B24" t="s">
         <v>4</v>
@@ -1542,320 +1545,320 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
+        <v>138</v>
+      </c>
+      <c r="B27" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
         <v>25</v>
       </c>
-      <c r="B27" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="1" t="s">
+      <c r="B28" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B30" s="1" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>30</v>
-      </c>
-      <c r="B30" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
         <v>31</v>
       </c>
-      <c r="B31" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A33" s="1" t="s">
+      <c r="B32" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B34" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
         <v>30</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B35" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
+    <row r="36" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
         <v>101</v>
       </c>
-      <c r="B35" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A37" s="1" t="s">
+      <c r="B36" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="B38" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
         <v>33</v>
       </c>
-      <c r="B38" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
+      <c r="B39" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
         <v>100</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B40" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A40" s="1"/>
-      <c r="B40" s="1"/>
-    </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A41" s="1" t="s">
+      <c r="A41" s="1"/>
+      <c r="B41" s="1"/>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B41" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
+      <c r="B42" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
         <v>30</v>
       </c>
-      <c r="B42" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A43"/>
-      <c r="B43"/>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A44" s="1" t="s">
+      <c r="B43" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A44"/>
+      <c r="B44"/>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A45" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B44" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
+      <c r="B45" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
         <v>30</v>
       </c>
-      <c r="B45" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A46"/>
-      <c r="B46"/>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A47" s="1" t="s">
+      <c r="B46" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A47"/>
+      <c r="B47"/>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A48" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B47" s="1" t="s">
+      <c r="B48" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
         <v>43</v>
-      </c>
-      <c r="B48" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
-        <v>30</v>
       </c>
       <c r="B49" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A51" s="1" t="s">
+    <row r="50" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>30</v>
+      </c>
+      <c r="B50" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A52" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B51" s="1" t="s">
+      <c r="B52" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
         <v>30</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B53" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="53" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A53"/>
-      <c r="B53"/>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A54" s="1" t="s">
+    <row r="54" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A54"/>
+      <c r="B54"/>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A55" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B54" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A55" t="s">
+      <c r="B55" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
         <v>30</v>
       </c>
-      <c r="B55" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="1" t="s">
+      <c r="B56" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B57" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A58" t="s">
+      <c r="B58" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
         <v>30</v>
       </c>
-      <c r="B58" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="1" t="s">
+      <c r="B59" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B60" s="1" t="s">
+      <c r="B61" s="1" t="s">
         <v>49</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A61" t="s">
-        <v>30</v>
-      </c>
-      <c r="B61" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>135</v>
+        <v>30</v>
       </c>
       <c r="B62" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="63" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="64" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="1" t="s">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>134</v>
+      </c>
+      <c r="B63" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="65" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B64" s="1" t="s">
+      <c r="B65" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="65" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="2" t="s">
+    <row r="66" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B65" s="2" t="s">
+      <c r="B66" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="67" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="1" t="s">
+    <row r="68" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B67" s="1" t="s">
+      <c r="B68" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="68" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="2" t="s">
+    <row r="69" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B68" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A69" s="2" t="s">
+      <c r="B69" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A70" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B69" s="2" t="s">
+      <c r="B70" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="71" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="1" t="s">
+    <row r="72" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A72" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B71" s="1" t="s">
+      <c r="B72" s="1" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A72" t="s">
-        <v>54</v>
-      </c>
-      <c r="B72" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B73" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
+        <v>55</v>
+      </c>
+      <c r="B74" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
         <v>30</v>
       </c>
-      <c r="B74" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A76" s="1" t="s">
+      <c r="B75" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A77" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B76" s="1" t="s">
+      <c r="B77" s="1" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A77" t="s">
-        <v>30</v>
-      </c>
-      <c r="B77" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>57</v>
+        <v>30</v>
       </c>
       <c r="B78" t="s">
         <v>21</v>
@@ -1863,201 +1866,209 @@
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
+        <v>57</v>
+      </c>
+      <c r="B79" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
         <v>59</v>
       </c>
-      <c r="B79" t="s">
+      <c r="B80" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="81" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A81" s="1" t="s">
+    <row r="82" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A82" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B81" s="1" t="s">
+      <c r="B82" s="1" t="s">
         <v>62</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A82" t="s">
-        <v>30</v>
-      </c>
-      <c r="B82" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
+        <v>30</v>
+      </c>
+      <c r="B83" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
         <v>61</v>
       </c>
-      <c r="B83" t="s">
+      <c r="B84" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A85" s="1" t="s">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A86" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B85" s="1" t="s">
+      <c r="B86" s="1" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A86" t="s">
-        <v>5</v>
-      </c>
-      <c r="B86" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B87" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B88" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B89" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="91" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A91" s="1" t="s">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
+        <v>8</v>
+      </c>
+      <c r="B90" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A92" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B91" s="1" t="s">
+      <c r="B92" s="1" t="s">
         <v>66</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A92" t="s">
-        <v>64</v>
-      </c>
-      <c r="B92" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B93" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B94" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="96" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A96" s="1" t="s">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
+        <v>67</v>
+      </c>
+      <c r="B95" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A97" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B96" s="1" t="s">
+      <c r="B97" s="1" t="s">
         <v>66</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A97" t="s">
-        <v>69</v>
-      </c>
-      <c r="B97" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B98" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="100" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A100" s="1" t="s">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A99" t="s">
+        <v>70</v>
+      </c>
+      <c r="B99" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A101" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B100" s="1" t="s">
+      <c r="B101" s="1" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A101" t="s">
-        <v>72</v>
-      </c>
-      <c r="B101" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
+        <v>72</v>
+      </c>
+      <c r="B102" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A103" t="s">
         <v>73</v>
       </c>
-      <c r="B102" t="s">
+      <c r="B103" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="104" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A104" s="1" t="s">
+    <row r="105" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A105" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B104" s="1" t="s">
+      <c r="B105" s="1" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A105" t="s">
-        <v>75</v>
-      </c>
-      <c r="B105" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
+        <v>75</v>
+      </c>
+      <c r="B106" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A107" t="s">
         <v>30</v>
       </c>
-      <c r="B106" t="s">
+      <c r="B107" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="108" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A108" s="1" t="s">
+    <row r="109" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A109" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B108" s="1" t="s">
+      <c r="B109" s="1" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A109" t="s">
-        <v>77</v>
-      </c>
-      <c r="B109" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
+        <v>77</v>
+      </c>
+      <c r="B110" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A111" t="s">
         <v>30</v>
       </c>
-      <c r="B110" t="s">
+      <c r="B111" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Input Color Basic Features
</commit_message>
<xml_diff>
--- a/Estimation du temps de travail.xlsx
+++ b/Estimation du temps de travail.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thiba\Documents\Projet\ArrakisNG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3689C03D-3234-48F5-A260-FDC5993B28FB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{481F6BA4-D039-4902-AB95-40FFA4901699}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -465,10 +465,10 @@
     <t>Principale, Scondaire</t>
   </si>
   <si>
-    <t>Export des fichiers SCSS + fonction de génération de thème</t>
-  </si>
-  <si>
     <t>Fonction de tri et de recherche</t>
+  </si>
+  <si>
+    <t>Fonction de création de thèmes</t>
   </si>
 </sst>
 </file>
@@ -1349,7 +1349,7 @@
   <dimension ref="A1:D111"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1444,7 +1444,7 @@
         <v>18</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>17</v>
+        <v>66</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -1457,7 +1457,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B13" t="s">
         <v>17</v>
@@ -1545,7 +1545,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B27" t="s">
         <v>22</v>

</xml_diff>